<commit_message>
update with MDE data
</commit_message>
<xml_diff>
--- a/Data/Original_Brown_etal/feeding_ecology_species.xlsx
+++ b/Data/Original_Brown_etal/feeding_ecology_species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/KK_etal_PFAS_food_web_model/Data/Original_Brown_etal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDA6714-B185-774F-8629-05DE9EF28E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5295BDDC-D7D0-2A46-B7EC-9FC1C5F00885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{FCDC5B72-DEA5-2942-AFB7-614A6345B706}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>Species</t>
   </si>
@@ -67,42 +67,12 @@
     <t xml:space="preserve">SED </t>
   </si>
   <si>
-    <t xml:space="preserve">  #   Phy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Dac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Dar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Fal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Bas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Mad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Pum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #   Swa</t>
-  </si>
-  <si>
     <t># JBA spring</t>
   </si>
   <si>
     <t xml:space="preserve">  # foodWeb = list(</t>
   </si>
   <si>
-    <t xml:space="preserve">  #     Phy</t>
-  </si>
-  <si>
     <t>foodWeb</t>
   </si>
   <si>
@@ -116,27 +86,6 @@
   </si>
   <si>
     <t>Bas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Mad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Dar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Pum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Swa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Chu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  #  Kil</t>
   </si>
   <si>
     <t>Rosyside Dace</t>
@@ -501,18 +450,6 @@
   </si>
   <si>
     <t>Benthopelagic invertivore/herbivore</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>demersal</t>
-  </si>
-  <si>
-    <t>small fish, insectivore</t>
-  </si>
-  <si>
-    <t>med size</t>
   </si>
   <si>
     <t>lots of insects, etc</t>
@@ -882,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -985,6 +922,33 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1038,24 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1371,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C4522E-F2E9-F14C-9CD6-F6AF3754642D}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1382,11 +1328,12 @@
     <col min="1" max="1" width="22" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" style="33" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="9"/>
+    <col min="4" max="4" width="20.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="54.6640625" style="33" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1396,407 +1343,463 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A2" s="45" t="s">
+      <c r="F1" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="55"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="56"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="76" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="52"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="46"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" ht="61" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A5" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="51" t="s">
+      <c r="F11" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="47"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="49"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="76" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="31" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A11" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="61" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A14" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="46" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A17" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="39" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="46"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" ht="46" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="46"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="46"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="46" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A26" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="B26" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="36"/>
+      <c r="E26" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="46"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="47"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A29" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="D29" s="36"/>
+      <c r="E29" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A20" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="39" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="47"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A32" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="B32" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="36"/>
+      <c r="E32" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" s="46"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="37"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A23" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="42" t="s">
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="47"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="37"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="59" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A26" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="37"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="38"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A29" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="37"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="A32" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="37"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="38"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
-      <c r="D35" s="32"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -1813,12 +1816,13 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1829,7 +1833,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1837,7 +1841,7 @@
     <col min="2" max="2" width="8.1640625" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="8.1640625" style="57" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" style="42" customWidth="1"/>
     <col min="14" max="14" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1849,42 +1853,39 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -1913,25 +1914,25 @@
       <c r="K2" s="5">
         <v>0</v>
       </c>
-      <c r="L2" s="58"/>
+      <c r="L2" s="43"/>
       <c r="M2">
         <f>SUM(B2:K2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" t="str">
         <f>CONCATENATE(A2," = c(",B2, ",", C2,",", D2, ",",E2, ",",F2, ",",G2, ",",H2, ",",I2, ",",J2, ",",K2, "),")</f>
-        <v>Phy = c(1,0,0,0,0,0,0,0,0,0),</v>
+        <v>Phy = c(0,0,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="6">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1957,22 +1958,22 @@
       <c r="K3" s="5">
         <v>0</v>
       </c>
-      <c r="L3" s="58"/>
+      <c r="L3" s="43"/>
       <c r="M3">
         <f t="shared" ref="M3:M10" si="0">SUM(B3:K3)</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N8" si="1">CONCATENATE(A3," = c(",B3, ",", C3,",", D3, ",",E3, ",",F3, ",",G3, ",",H3, ",",I3, ",",J3, ",",K3, "),")</f>
-        <v>Dac = c(0.5,0.4,0,0,0,0,0,0,0,0),</v>
+        <v>Bas = c(0.8,0.2,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C4" s="6">
         <v>0.6</v>
@@ -2001,26 +2002,26 @@
       <c r="K4" s="5">
         <v>0</v>
       </c>
-      <c r="L4" s="58"/>
+      <c r="L4" s="43"/>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="1"/>
-        <v>Dar = c(0.5,0.6,0,0,0,0,0,0,0,0),</v>
+        <v>Swa = c(0.3,0.6,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="6">
         <v>0.4</v>
       </c>
-      <c r="C5" s="6">
-        <v>0.6</v>
-      </c>
       <c r="D5" s="5">
         <v>0</v>
       </c>
@@ -2045,27 +2046,25 @@
       <c r="K5" s="5">
         <v>0</v>
       </c>
-      <c r="L5" s="58" t="s">
-        <v>117</v>
-      </c>
+      <c r="L5" s="43"/>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="1"/>
-        <v>Min = c(0.4,0.6,0,0,0,0,0,0,0,0),</v>
+        <v>Dac = c(0.5,0.4,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C6" s="6">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
@@ -2091,27 +2090,25 @@
       <c r="K6" s="5">
         <v>0</v>
       </c>
-      <c r="L6" s="58" t="s">
-        <v>118</v>
-      </c>
+      <c r="L6" s="43"/>
       <c r="M6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="1"/>
-        <v>Fal = c(0.5,0.5,0,0,0,0,0,0,0,0),</v>
+        <v>Min = c(0.4,0.6,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B7" s="3">
         <v>0.2</v>
       </c>
       <c r="C7" s="6">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -2123,7 +2120,7 @@
         <v>0.1</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
@@ -2135,39 +2132,39 @@
         <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="L7" s="58"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="43"/>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="1"/>
-        <v>Bas = c(0.2,0.4,0,0.1,0.1,0,0,0,0,0.2),</v>
+        <v>Fal = c(0.2,0.3,0,0.1,0.1,0.1,0,0,0,0),</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B8" s="3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C8" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="5">
         <v>0</v>
@@ -2181,34 +2178,34 @@
       <c r="K8" s="5">
         <v>0</v>
       </c>
-      <c r="L8" s="58"/>
+      <c r="L8" s="43"/>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="1"/>
-        <v>Mad = c(0.5,0.5,0,0,0,0,0,0,0,0),</v>
+        <v>Mad = c(0.2,0.3,0,0.1,0.1,0.1,0,0,0,0),</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="6">
         <v>0.3</v>
       </c>
-      <c r="C9" s="6">
-        <v>0.5</v>
-      </c>
       <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.1</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
       <c r="F9" s="5">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -2223,41 +2220,39 @@
         <v>0</v>
       </c>
       <c r="K9" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="L9" s="58" t="s">
-        <v>119</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L9" s="43"/>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="N9" t="str">
         <f>CONCATENATE(A9," = c(",B9, ",", C9,",", D9, ",",E9, ",",F9, ",",G9, ",",H9, ",",I9, ",",J9, ",",K9, "),")</f>
-        <v>Pum = c(0.3,0.5,0.1,0,0.05,0,0,0,0,0.05),</v>
+        <v>Dar = c(0.2,0.3,0,0.1,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C10" s="6">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G10" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H10" s="5">
         <v>0</v>
@@ -2271,59 +2266,59 @@
       <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="58"/>
+      <c r="L10" s="43"/>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N10" t="str">
         <f>CONCATENATE(A10," = c(",B10, ",", C10,",", D10, ",",E10, ",",F10, ",",G10, ",",H10, ",",I10, ",",J10, ",",K10, ")")</f>
-        <v>Swa = c(0.3,0.7,0,0,0,0,0,0,0,0)</v>
+        <v>Pum = c(0.2,0.2,0.1,0,0.1,0.1,0,0,0,0)</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="K13" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -2355,19 +2350,19 @@
       <c r="K14" s="5">
         <v>0</v>
       </c>
-      <c r="L14" s="58"/>
+      <c r="L14" s="43"/>
       <c r="M14">
         <f>SUM(B14:K14)</f>
         <v>1</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" ref="N14:N21" si="2">CONCATENATE(A14," = c(",B14, ",", C14,",", D14, ",",E14, ",",F14, ",",G14, ",",H14, ",",I14, ",",J14, ",",K14, "),")</f>
+        <f>CONCATENATE(A14," = c(",B14, ",", C14,",", D14, ",",E14, ",",F14, ",",G14, ",",H14, ",",I14, ",",J14, ",",K14, "),")</f>
         <v>Phy = c(1,0,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3">
         <v>0.4</v>
@@ -2399,25 +2394,25 @@
       <c r="K15" s="5">
         <v>0</v>
       </c>
-      <c r="L15" s="58"/>
+      <c r="L15" s="43"/>
       <c r="M15">
-        <f t="shared" ref="M15:M22" si="3">SUM(B15:K15)</f>
+        <f t="shared" ref="M15:M22" si="2">SUM(B15:K15)</f>
         <v>1</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="N14:N20" si="3">CONCATENATE(A15," = c(",B15, ",", C15,",", D15, ",",E15, ",",F15, ",",G15, ",",H15, ",",I15, ",",J15, ",",K15, "),")</f>
         <v>Kil = c(0.4,0.6,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B16" s="3">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="C16" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -2443,21 +2438,21 @@
       <c r="K16" s="5">
         <v>0</v>
       </c>
-      <c r="L16" s="58" t="s">
-        <v>120</v>
+      <c r="L16" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="N16" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="2"/>
-        <v>Chu = c(0.7,0.3,0,0,0,0,0,0,0,0),</v>
+        <v>Swa = c(0.3,0.5,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3">
         <v>0.5</v>
@@ -2489,22 +2484,22 @@
       <c r="K17" s="5">
         <v>0</v>
       </c>
-      <c r="L17" s="58"/>
+      <c r="L17" s="43"/>
       <c r="M17">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="N17" t="str">
         <f t="shared" si="3"/>
-        <v>0.9</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="2"/>
         <v>Dac = c(0.5,0.4,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C18" s="6">
         <v>0.6</v>
@@ -2533,37 +2528,37 @@
       <c r="K18" s="5">
         <v>0</v>
       </c>
-      <c r="L18" s="58"/>
+      <c r="L18" s="43"/>
       <c r="M18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="3"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="2"/>
-        <v>Dar = c(0.5,0.6,0,0,0,0,0,0,0,0),</v>
+        <v>Min = c(0.4,0.6,0,0,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B19" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C19" s="6">
         <v>0.4</v>
       </c>
-      <c r="C19" s="6">
-        <v>0.6</v>
-      </c>
       <c r="D19" s="5">
         <v>0</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G19" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
@@ -2577,22 +2572,22 @@
       <c r="K19" s="5">
         <v>0</v>
       </c>
-      <c r="L19" s="58"/>
+      <c r="L19" s="43"/>
       <c r="M19">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="2"/>
-        <v>Min = c(0.4,0.6,0,0,0,0,0,0,0,0),</v>
+        <v>Mad = c(0.3,0.4,0,0.1,0.1,0.1,0,0,0,0),</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C20" s="6">
         <v>0.5</v>
@@ -2601,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -2621,28 +2616,28 @@
       <c r="K20" s="5">
         <v>0</v>
       </c>
-      <c r="L20" s="58"/>
+      <c r="L20" s="43"/>
       <c r="M20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N20" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="2"/>
-        <v>Mad = c(0.5,0.5,0,0,0,0,0,0,0,0),</v>
+        <v>Dar = c(0.4,0.5,0,0.1,0,0,0,0,0,0),</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B21" s="3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C21" s="6">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -2651,7 +2646,7 @@
         <v>0.1</v>
       </c>
       <c r="G21" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
@@ -2663,39 +2658,39 @@
         <v>0</v>
       </c>
       <c r="K21" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="L21" s="58"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="43"/>
       <c r="M21">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.7</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="2"/>
-        <v>Pum = c(0.3,0.5,0,0,0.1,0,0,0,0,0.1),</v>
+        <f>CONCATENATE(A21," = c(",B21, ",", C21,",", D21, ",",E21, ",",F21, ",",G21, ",",H21, ",",I21, ",",J21, ",",K21, "),")</f>
+        <v>Pum = c(0.2,0.2,0.1,0,0.1,0.1,0,0,0,0),</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="6">
         <v>0.2</v>
       </c>
-      <c r="C22" s="6">
-        <v>0.8</v>
-      </c>
       <c r="D22" s="5">
         <v>0</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H22" s="5">
         <v>0</v>
@@ -2709,39 +2704,39 @@
       <c r="K22" s="4">
         <v>0</v>
       </c>
-      <c r="L22" s="58"/>
+      <c r="L22" s="43"/>
       <c r="M22">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
       </c>
       <c r="N22" t="str">
         <f>CONCATENATE(A22," = c(",B22, ",", C22,",", D22, ",",E22, ",",F22, ",",G22, ",",H22, ",",I22, ",",J22, ",",K22, ")")</f>
-        <v>Swa = c(0.2,0.8,0,0,0,0,0,0,0,0)</v>
+        <v>Chu = c(0.5,0.2,0,0.1,0.1,0.1,0,0,0,0)</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -2769,13 +2764,13 @@
     </row>
     <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B29" s="3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="C29" s="6">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -2792,12 +2787,12 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" ref="H29:H30" si="5">CONCATENATE(A29, " = c(",B29, ",",C29, ",",D29, ",",E29, ",",F29, "),")</f>
-        <v>Pry = c(0.4,0.6,0,0,0),</v>
+        <v>Pry = c(0.7,0.3,0,0,0),</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B30" s="3">
         <v>0.1</v>
@@ -2825,16 +2820,16 @@
     </row>
     <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B31" s="3">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C31" s="6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D31" s="5">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="E31" s="5">
         <v>0.1</v>
@@ -2848,7 +2843,7 @@
       </c>
       <c r="H31" t="str">
         <f>CONCATENATE(A31, " = c(",B31, ",",C31, ",",D31, ",",E31, ",",F31, ")")</f>
-        <v>Bas = c(0.3,0.3,0.3,0.1,0)</v>
+        <v>Bas = c(0.1,0.1,0.7,0.1,0)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>